<commit_message>
Fase 3, informe final y scripts de datos V2
</commit_message>
<xml_diff>
--- a/Equipo07/Fase 2/Evidencias_Proyecto/Evidencias_de_documentacion/Sprint_Backlog_Actividades_Horas_DFF.xlsx
+++ b/Equipo07/Fase 2/Evidencias_Proyecto/Evidencias_de_documentacion/Sprint_Backlog_Actividades_Horas_DFF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotas\Desktop\Capstone_Equipo07_Fase1\Equipo07\Fase 2\Evidencias_Proyecto\Evidencias_de_documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C79660F-C913-4B13-9492-A05B77FAB5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEBB432-1F2B-421B-9ACC-60CE23C75C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product_Backlog_tareas" sheetId="1" r:id="rId1"/>
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,7 +896,7 @@
       <c r="B2" s="4"/>
       <c r="C2" s="3">
         <f>SUM(D5:D78)</f>
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1136,7 +1136,7 @@
         <v>41</v>
       </c>
       <c r="D20" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>